<commit_message>
Get everything ready for PBET 2022 testing
</commit_message>
<xml_diff>
--- a/data-raw/PBET_dict.xlsx
+++ b/data-raw/PBET_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/PBET/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD0A81A-1915-2A46-808F-803668A98A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBEDA3F-3FD3-954E-8BB8-2AD4B20787B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1960" windowWidth="35840" windowHeight="20720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="206">
   <si>
     <t>key</t>
   </si>
@@ -704,6 +704,36 @@
   </si>
   <si>
     <t>In this task we’ll ask you to play back a few notes and melodies that we play to you. The test will start easy and get very hard. Just do your best and have fun!</t>
+  </si>
+  <si>
+    <t>welcome_message</t>
+  </si>
+  <si>
+    <t>test_instructions_2.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can have up to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sie erhalten bis zu </t>
+  </si>
+  <si>
+    <t>test_instructions_2.1.2</t>
+  </si>
+  <si>
+    <t>goes to get the melody as best you can.</t>
+  </si>
+  <si>
+    <t>Versuche um Ihr bestmöglichstes Resultat zu erreichen.</t>
+  </si>
+  <si>
+    <t>test_instructions_2.1.1.forced</t>
+  </si>
+  <si>
+    <t>You will have</t>
+  </si>
+  <si>
+    <t>Sie erhalten</t>
   </si>
 </sst>
 </file>
@@ -817,7 +847,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -846,6 +876,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1064,10 +1098,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1089,765 +1123,812 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>191</v>
+      <c r="A2" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="2" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A4" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A5" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>192</v>
+        <v>121</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A7" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="2" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A8" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A9" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A10" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>81</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>26</v>
+      <c r="A12" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>175</v>
+        <v>126</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>29</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A14" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>84</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>75</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
+      <c r="A17" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>37</v>
+      <c r="A18" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
+        <v>136</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>108</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>42</v>
+      <c r="A20" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>45</v>
+      <c r="A21" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>48</v>
+      <c r="A22" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>51</v>
+      <c r="A23" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>58</v>
+      <c r="A26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>60</v>
+      <c r="A27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>62</v>
+      <c r="A28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A29" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>64</v>
+      <c r="A29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A30" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>66</v>
+      <c r="A30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>68</v>
+      <c r="A31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A32" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>70</v>
+      <c r="A32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A33" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34" s="17" t="s">
+      <c r="A33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="13">
+      <c r="A34" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="13">
+      <c r="A35" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A36" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A37" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B37" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C37" s="17" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A37" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>81</v>
+        <v>191</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>86</v>
+      <c r="A39" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A40" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>89</v>
+      <c r="A40" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A41" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>92</v>
+      <c r="A41" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>94</v>
+        <v>78</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A43" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>98</v>
+      <c r="A43" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A44" s="2" t="s">
-        <v>99</v>
+      <c r="A44" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>106</v>
+        <v>16</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>107</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>109</v>
+        <v>19</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>113</v>
+        <v>22</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>116</v>
+        <v>25</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1">
       <c r="A50" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>118</v>
+        <v>27</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A51" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>122</v>
+      <c r="A51" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A52" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>9</v>
+      <c r="A52" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A53" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>124</v>
+      <c r="A53" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>125</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" customHeight="1">
       <c r="A54" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>127</v>
+        <v>13</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" customHeight="1">
       <c r="A55" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" customHeight="1">
       <c r="A56" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A57" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>137</v>
+      <c r="A57" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A58" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>139</v>
+      <c r="A58" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A59" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>142</v>
+      <c r="A59" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A60" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>145</v>
+      <c r="A60" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A61" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>148</v>
+      <c r="A61" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A62" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>151</v>
+      <c r="A62" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A63" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>154</v>
+      <c r="A63" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A64" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="B64" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="13">
-      <c r="A65" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="13">
-      <c r="A66" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="13">
-      <c r="A67" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B67" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C67" s="13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="13">
-      <c r="A68" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B68" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="13">
-      <c r="A69" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="C69" s="13" t="s">
-        <v>172</v>
+      <c r="A64" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A65" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C65" s="24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A66" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A67" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A68" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A69" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A70" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="B70" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>190</v>
+      <c r="A70" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A71" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A72" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B72" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A73" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A74" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C74">
+    <sortCondition ref="A1:A74"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update with new musicassessr_aws setup
</commit_message>
<xml_diff>
--- a/data-raw/PBET_dict.xlsx
+++ b/data-raw/PBET_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/Downloads/retranslations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/PBET/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159DD095-4E1F-364F-A5B5-948F93E04B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF13E694-E1EA-BD45-9B2F-870965DC5E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="520" windowWidth="35840" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="210">
   <si>
     <t>key</t>
   </si>
@@ -740,6 +740,12 @@
   </si>
   <si>
     <t>Andere (bitte benennen Sie es)</t>
+  </si>
+  <si>
+    <t>test_instructions_4</t>
+  </si>
+  <si>
+    <t>For best results, do not sing along with your instrument. Just play!</t>
   </si>
 </sst>
 </file>
@@ -1099,10 +1105,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="172" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="172" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1849,86 +1855,97 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1">
+    <row r="68" spans="1:3" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="A68" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A69" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B69" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A69" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C69" s="16" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" customHeight="1">
       <c r="A70" s="16" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.75" customHeight="1">
       <c r="A71" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A72" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A72" s="21" t="s">
+    <row r="73" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A73" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="B72" s="22" t="s">
+      <c r="B73" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C73" s="21" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A73" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" customHeight="1">
       <c r="A74" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A75" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>206</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C74">
-    <sortCondition ref="A1:A74"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C75">
+    <sortCondition ref="A1:A75"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update to match new "paradigm" feature in musicassessr and various other updates to support DB usage.
</commit_message>
<xml_diff>
--- a/data-raw/PBET_dict.xlsx
+++ b/data-raw/PBET_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/PBET/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF13E694-E1EA-BD45-9B2F-870965DC5E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85115E14-8E1E-E749-B003-310CD6E8A036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="520" windowWidth="35840" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="3620" windowWidth="35840" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="211">
   <si>
     <t>key</t>
   </si>
@@ -746,6 +746,9 @@
   </si>
   <si>
     <t>For best results, do not sing along with your instrument. Just play!</t>
+  </si>
+  <si>
+    <t>it</t>
   </si>
 </sst>
 </file>
@@ -853,40 +856,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1105,10 +1102,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="172" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="172" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1118,7 +1115,7 @@
     <col min="3" max="3" width="125.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1126,820 +1123,1045 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A2" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A4" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>110</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A5" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A6" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A7" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A8" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A9" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A10" s="16" t="s">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A10" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>115</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A11" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A12" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>144</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A13" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A14" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A15" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A16" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A17" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A18" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A19" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A20" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>153</v>
       </c>
       <c r="C20" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A21" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A22" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="11" t="s">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A23" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A25" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A26" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A27" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A28" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A29" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A30" s="5" t="s">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A30" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A31" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A32" s="2" t="s">
+      <c r="D31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A32" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A33" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="13">
-      <c r="A34" s="11" t="s">
+    <row r="34" spans="1:4" ht="13">
+      <c r="A34" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="13">
-      <c r="A35" s="10" t="s">
+    <row r="35" spans="1:4" ht="13">
+      <c r="A35" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>138</v>
       </c>
       <c r="C35" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="10" t="s">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A36" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A37" s="16" t="s">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A37" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="17" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A38" t="s">
         <v>182</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A39" s="19" t="s">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A39" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A40" s="19" t="s">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A40" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="D40" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A41" s="16" t="s">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A41" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A42" s="2" t="s">
+    <row r="42" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A42" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A43" s="10" t="s">
+    <row r="43" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A43" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>141</v>
       </c>
       <c r="C43" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A44" s="17" t="s">
+    <row r="44" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A44" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A45" s="2" t="s">
+    <row r="45" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A45" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A46" s="2" t="s">
+    <row r="46" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A46" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A47" s="2" t="s">
+    <row r="47" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A47" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A48" s="2" t="s">
+    <row r="48" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A48" t="s">
         <v>22</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A49" s="2" t="s">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A49" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D49" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A50" s="2" t="s">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A50" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D50" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A51" s="2" t="s">
+    <row r="51" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A51" t="s">
         <v>164</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A52" s="8" t="s">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A52" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A53" s="2" t="s">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A53" t="s">
         <v>30</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A54" s="2" t="s">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A54" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A55" t="s">
         <v>124</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D55" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A56" s="2" t="s">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A56" t="s">
         <v>121</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D56" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A57" s="16" t="s">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A57" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A58" s="2" t="s">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A58" t="s">
         <v>76</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A59" s="16" t="s">
+      <c r="D58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A59" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C59" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" s="15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A60" s="2" t="s">
+    <row r="60" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A60" t="s">
         <v>83</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A61" s="2" t="s">
+    <row r="61" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A61" t="s">
         <v>86</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C61" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A62" s="2" t="s">
+    <row r="62" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A62" t="s">
         <v>89</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C62" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D62" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A63" s="23" t="s">
+    <row r="63" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A63" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="B63" s="24" t="s">
+      <c r="B63" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="C63" s="23" t="s">
+      <c r="C63" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="D63" s="17" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A64" s="23" t="s">
+    <row r="64" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A64" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="B64" s="24" t="s">
+      <c r="B64" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="C64" s="23" t="s">
+      <c r="C64" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D64" s="17" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A65" s="23" t="s">
+    <row r="65" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A65" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="B65" s="24" t="s">
+      <c r="B65" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="C65" s="23" t="s">
+      <c r="C65" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D65" s="17" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A66" s="2" t="s">
+    <row r="66" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A66" t="s">
         <v>92</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D66" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A67" s="2" t="s">
+    <row r="67" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A67" t="s">
         <v>95</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D67" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="2" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A68" s="2" t="s">
+    <row r="68" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A68" t="s">
         <v>208</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A69" s="2" t="s">
+      <c r="D68" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A69" t="s">
         <v>3</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C69" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A70" s="16" t="s">
+    <row r="70" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A70" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B70" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="16" t="s">
+      <c r="C70" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D70" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A71" s="16" t="s">
+    <row r="71" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A71" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C71" s="16" t="s">
+      <c r="C71" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D71" s="15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A72" s="16" t="s">
+    <row r="72" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A72" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" t="s">
         <v>116</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" t="s">
+        <v>116</v>
+      </c>
+      <c r="D72" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A73" s="21" t="s">
+    <row r="73" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A73" t="s">
         <v>187</v>
       </c>
-      <c r="B73" s="22" t="s">
+      <c r="B73" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="21" t="s">
+      <c r="C73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A74" s="2" t="s">
+    <row r="74" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A74" t="s">
         <v>33</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A75" s="2" t="s">
+    <row r="75" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A75" t="s">
         <v>81</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D75" t="s">
         <v>206</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to support API mode testing
</commit_message>
<xml_diff>
--- a/data-raw/PBET_dict.xlsx
+++ b/data-raw/PBET_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/PBET/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B98683-FF3B-0842-B40A-541CBF8614C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202DA7E7-577B-9848-A3E7-87CC2129718B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="35840" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4280" windowWidth="35840" windowHeight="20720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="217">
   <si>
     <t>key</t>
   </si>
@@ -330,12 +330,6 @@
   </si>
   <si>
     <t>In diesem Test hören Sie eine Melodie.</t>
-  </si>
-  <si>
-    <t>test_instructions_1.2</t>
-  </si>
-  <si>
-    <t>You must perform this melody back on your instrument as accurately as you can.</t>
   </si>
   <si>
     <t>Geben Sie die Melodie so akkurat wie möglich auf Ihrem Instrument wieder.</t>
@@ -752,6 +746,27 @@
   </si>
   <si>
     <t>lv</t>
+  </si>
+  <si>
+    <t>You can have up to 3 attempts to get the melody as best you can.</t>
+  </si>
+  <si>
+    <t>attempts to get the melody as best you can.</t>
+  </si>
+  <si>
+    <t>You will be able to take as many attempts as you like.</t>
+  </si>
+  <si>
+    <t>In this test, you will hear some melodies.</t>
+  </si>
+  <si>
+    <t>You must perform these melodies back on your instrument as accurately as you can.</t>
+  </si>
+  <si>
+    <t>test_instructions_1.2</t>
+  </si>
+  <si>
+    <t>test_instructions_2.1.infinite</t>
   </si>
 </sst>
 </file>
@@ -1105,10 +1120,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1126,18 +1141,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>61</v>
@@ -1154,75 +1169,75 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" t="s">
-        <v>111</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" t="s">
-        <v>105</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>65</v>
@@ -1239,7 +1254,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>57</v>
@@ -1256,36 +1271,36 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>181</v>
-      </c>
       <c r="E9" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1">
@@ -1299,7 +1314,7 @@
         <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>78</v>
@@ -1307,41 +1322,41 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>145</v>
-      </c>
       <c r="E12" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
         <v>118</v>
       </c>
-      <c r="B13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
-      </c>
       <c r="E13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>55</v>
@@ -1367,7 +1382,7 @@
         <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>80</v>
@@ -1384,7 +1399,7 @@
         <v>73</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>73</v>
@@ -1392,121 +1407,121 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" t="s">
-        <v>131</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" t="s">
-        <v>128</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>154</v>
-      </c>
       <c r="E20" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="E21" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>160</v>
-      </c>
       <c r="E22" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>163</v>
-      </c>
       <c r="E23" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
@@ -1520,7 +1535,7 @@
         <v>38</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>38</v>
@@ -1545,19 +1560,19 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" t="s">
-        <v>100</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1">
@@ -1622,7 +1637,7 @@
         <v>46</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>46</v>
@@ -1681,58 +1696,58 @@
     </row>
     <row r="34" spans="1:5" ht="13">
       <c r="A34" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>151</v>
-      </c>
       <c r="E34" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="13">
       <c r="A35" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="E35" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>148</v>
-      </c>
       <c r="E36" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>71</v>
@@ -1741,7 +1756,7 @@
         <v>71</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>71</v>
@@ -1749,7 +1764,7 @@
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>6</v>
@@ -1766,41 +1781,41 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>186</v>
-      </c>
       <c r="C39" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D39" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1">
       <c r="A40" s="18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D40" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>53</v>
@@ -1834,36 +1849,36 @@
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>142</v>
-      </c>
       <c r="E43" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1">
       <c r="A44" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D44" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1">
@@ -1939,16 +1954,16 @@
         <v>25</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D49" t="s">
         <v>26</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" customHeight="1">
@@ -1956,21 +1971,21 @@
         <v>27</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D50" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="A51" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>28</v>
@@ -1987,19 +2002,19 @@
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="A52" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B52" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>136</v>
-      </c>
       <c r="E52" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1">
@@ -2038,41 +2053,41 @@
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D55" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1">
       <c r="A56" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56" t="s">
         <v>121</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D56" t="s">
-        <v>123</v>
-      </c>
       <c r="E56" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1">
       <c r="A57" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B57" s="15" t="s">
         <v>59</v>
@@ -2106,7 +2121,7 @@
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1">
       <c r="A59" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B59" s="15" t="s">
         <v>63</v>
@@ -2125,8 +2140,8 @@
       <c r="A60" t="s">
         <v>83</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>84</v>
+      <c r="B60" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>84</v>
@@ -2134,268 +2149,285 @@
       <c r="D60" t="s">
         <v>85</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>84</v>
+      <c r="E60" s="20" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A61" t="s">
+      <c r="A61" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="D61" t="s">
         <v>86</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="E61" s="20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A62" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="B62" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A62" t="s">
+      <c r="D62" t="s">
         <v>89</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D62" t="s">
-        <v>91</v>
-      </c>
       <c r="E62" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1">
       <c r="A63" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D63" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="B63" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="C63" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>190</v>
-      </c>
       <c r="E63" s="20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1">
       <c r="A64" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D64" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="B64" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="C64" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>196</v>
-      </c>
       <c r="E64" s="20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1">
       <c r="A65" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="D65" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="B65" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="C65" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>193</v>
-      </c>
       <c r="E65" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A66" t="s">
-        <v>92</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D66" t="s">
-        <v>94</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>93</v>
+      <c r="A66" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1">
       <c r="A67" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D67" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1">
       <c r="A68" t="s">
-        <v>208</v>
+        <v>93</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>209</v>
+        <v>94</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>209</v>
+        <v>94</v>
+      </c>
+      <c r="D68" t="s">
+        <v>95</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>209</v>
+        <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1">
       <c r="A69" t="s">
+        <v>206</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A70" t="s">
         <v>3</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>5</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A70" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D70" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E70" s="15" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1">
       <c r="A71" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1">
       <c r="A72" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="B72" t="s">
-        <v>116</v>
-      </c>
-      <c r="C72" t="s">
-        <v>116</v>
-      </c>
-      <c r="D72" t="s">
-        <v>117</v>
-      </c>
-      <c r="E72" t="s">
-        <v>116</v>
+        <v>174</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A73" t="s">
-        <v>187</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>6</v>
+      <c r="A73" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B73" t="s">
+        <v>114</v>
+      </c>
+      <c r="C73" t="s">
+        <v>114</v>
       </c>
       <c r="D73" t="s">
-        <v>7</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>6</v>
+        <v>115</v>
+      </c>
+      <c r="E73" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>33</v>
-      </c>
-      <c r="B74" t="s">
-        <v>33</v>
-      </c>
-      <c r="C74" t="s">
-        <v>33</v>
+        <v>185</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>34</v>
-      </c>
-      <c r="E74" t="s">
-        <v>33</v>
+        <v>7</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15.75" customHeight="1">
       <c r="A75" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A76" t="s">
         <v>81</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D75" t="s">
-        <v>206</v>
-      </c>
-      <c r="E75" s="2" t="s">
+      <c r="D76" t="s">
+        <v>204</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C75">
-    <sortCondition ref="A1:A75"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C76">
+    <sortCondition ref="A1:A76"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>